<commit_message>
Fix for best fit breaking games when someone left. Scenario names and descriptions now always the correct language in scenario select. Full rooms no longer shown in room list. Localization fixes for UI and tutorial.
</commit_message>
<xml_diff>
--- a/Simulation/PlayGen.ITAlert.Simulation.Scenario.Localization/ScenarioLocalization.xlsx
+++ b/Simulation/PlayGen.ITAlert.Simulation.Scenario.Localization/ScenarioLocalization.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="157">
   <si>
     <t>Key</t>
   </si>
@@ -77,10 +77,6 @@
     <t>Tutorial1_Frame3</t>
   </si>
   <si>
-    <t xml:space="preserve">Your current destination will flash to indicate that you are being routed to that location. 
-</t>
-  </si>
-  <si>
     <t>Tutorial1_Frame4</t>
   </si>
   <si>
@@ -193,19 +189,10 @@
 Use the Scanner to reveal the Virus.</t>
   </si>
   <si>
-    <t xml:space="preserve">Een Virus heeft het linker werkstation geïnfecteerd. Het maakt het werkstation langzamer en ook de netwerk verbindingen aan dit werkstation worden langzamer.
-Gebruik de Scanner om het Virus zichtbaar te maken...
-</t>
-  </si>
-  <si>
     <t>Tutorial2_Frame4</t>
   </si>
   <si>
     <t>Now that the Virus is revealed you need to obtain a sample for analysis.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nu het Virus zichtbaar is, kunnen we een sample nemen om te analyseren.
-</t>
   </si>
   <si>
     <t>Tutorial2_Frame5</t>
@@ -215,11 +202,6 @@
 Go to the Analysis Workstation and collect the Capture tool.</t>
   </si>
   <si>
-    <t xml:space="preserve">Om een sample te nemen van een Virus gebruik je het Capture gereedschap dat zojuist is geïnstalleerd op het Analyse Werkstation.
-Klik op het Analyse Werkstation and als je daar bent, pak dan het Capture gereedschap op...
-</t>
-  </si>
-  <si>
     <t>Tutorial2_Frame6</t>
   </si>
   <si>
@@ -290,15 +272,7 @@
 Your Red Antivirus won't work against this.</t>
   </si>
   <si>
-    <t xml:space="preserve">Een nieuw Virus is binnengedrongen op Werkstation [10]
-</t>
-  </si>
-  <si>
     <t>Tutorial2_Frame14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repeat the previous process to eliminate the infection.
-</t>
   </si>
   <si>
     <t>Dit is een ander type virus, je Rode Antivirus zal hier niet tegen werken.
@@ -485,11 +459,6 @@
 Produce a red and a green Antivirus and bring them to the Workstation [10]</t>
   </si>
   <si>
-    <t xml:space="preserve">Om deze infectie te verwijderen, heb je een Antivirus nodig van elk aanwezig genoom waaruit het Virus is opgebouwd.
-Produceer een Rood en Groen Antivirus en breng ze naar het geïnfecteerde werkstation.
-</t>
-  </si>
-  <si>
     <t>Tutorial4_Frame9</t>
   </si>
   <si>
@@ -505,11 +474,6 @@
 Navigate to Workstation [00] by clicking on it.</t>
   </si>
   <si>
-    <t xml:space="preserve">Je bevindt je op Werkstation [10].
-Navigeer naar een ander werkstation door er op te klikken...
-</t>
-  </si>
-  <si>
     <t>Je huidige bestemming knippert om aan te geven dat je naar die locatie op weg bent.</t>
   </si>
   <si>
@@ -550,6 +514,31 @@
   </si>
   <si>
     <t>De Capture tool nog een activeren vangt het volgende genome in het Virus, en dat gaat zo rond.</t>
+  </si>
+  <si>
+    <t>Je bevindt je op Werkstation [10].
+Navigeer naar een ander werkstation door er op te klikken…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your current destination will flash to indicate that you are being routed to that location. </t>
+  </si>
+  <si>
+    <t>Nu het Virus zichtbaar is, kunnen we een sample nemen om te analyseren.</t>
+  </si>
+  <si>
+    <t>Een Virus heeft het linker werkstation geïnfecteerd. Het maakt het werkstation langzamer en ook de netwerk verbindingen aan dit werkstation worden langzamer.
+Gebruik de Scanner om het Virus zichtbaar te maken…</t>
+  </si>
+  <si>
+    <t>Om een sample te nemen van een Virus gebruik je het Capture gereedschap dat zojuist is geïnstalleerd op het Analyse Werkstation.
+Klik op het Analyse Werkstation and als je daar bent, pak dan het Capture gereedschap op…</t>
+  </si>
+  <si>
+    <t>Repeat the previous process to eliminate the infection.</t>
+  </si>
+  <si>
+    <t>Om deze infectie te verwijderen, heb je een Antivirus nodig van elk aanwezig genoom waaruit het Virus is opgebouwd.
+Produceer een Rood en Groen Antivirus en breng ze naar het geïnfecteerde werkstation.</t>
   </si>
 </sst>
 </file>
@@ -952,10 +941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1101,207 +1090,214 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>19</v>
+        <v>151</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+      <c r="B18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>41</v>
+        <v>42</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
+        <v>44</v>
+      </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
-        <v>46</v>
+      <c r="A21" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="9" t="s">
-        <v>52</v>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>54</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
@@ -1312,407 +1308,401 @@
         <v>56</v>
       </c>
       <c r="C24" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="25" spans="1:26" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
+      <c r="B25" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="7" t="s">
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
+      <c r="B26" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C26" s="7" t="s">
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
+      <c r="B27" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C28" s="7" t="s">
+    </row>
+    <row r="29" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
+      <c r="B29" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="7" t="s">
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
+      <c r="B30" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C30" s="7" t="s">
+    </row>
+    <row r="31" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
+      <c r="B31" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>77</v>
-      </c>
       <c r="C31" s="7" t="s">
-        <v>78</v>
+        <v>147</v>
       </c>
     </row>
     <row r="32" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B32" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>80</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="34" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C34" s="7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>156</v>
-      </c>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
+      <c r="T35" s="6"/>
+      <c r="U35" s="6"/>
+      <c r="V35" s="6"/>
+      <c r="W35" s="6"/>
+      <c r="X35" s="6"/>
+      <c r="Y35" s="6"/>
+      <c r="Z35" s="6"/>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B37" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C37" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="6"/>
-      <c r="T36" s="6"/>
-      <c r="U36" s="6"/>
-      <c r="V36" s="6"/>
-      <c r="W36" s="6"/>
-      <c r="X36" s="6"/>
-      <c r="Y36" s="6"/>
-      <c r="Z36" s="6"/>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A37" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B42" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C42" s="7" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="42" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>112</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="6"/>
+      <c r="R43" s="6"/>
+      <c r="S43" s="6"/>
+      <c r="T43" s="6"/>
+      <c r="U43" s="6"/>
+      <c r="V43" s="6"/>
+      <c r="W43" s="6"/>
+      <c r="X43" s="6"/>
+      <c r="Y43" s="6"/>
+      <c r="Z43" s="6"/>
     </row>
     <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
-      <c r="L44" s="6"/>
-      <c r="M44" s="6"/>
-      <c r="N44" s="6"/>
-      <c r="O44" s="6"/>
-      <c r="P44" s="6"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="6"/>
-      <c r="S44" s="6"/>
-      <c r="T44" s="6"/>
-      <c r="U44" s="6"/>
-      <c r="V44" s="6"/>
-      <c r="W44" s="6"/>
-      <c r="X44" s="6"/>
-      <c r="Y44" s="6"/>
-      <c r="Z44" s="6"/>
+        <v>112</v>
+      </c>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B47" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C47" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A47" s="4" t="s">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B48" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C48" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A48" s="4" t="s">
+    <row r="49" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B49" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C49" s="7" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A49" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B51" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C51" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="51" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
+      <c r="B52" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="C52" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A53" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="B53" s="7" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
+      <c r="C53" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B52" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="53" spans="1:26" ht="51" x14ac:dyDescent="0.2">
-      <c r="A53" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="54" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="6"/>
-      <c r="J54" s="6"/>
-      <c r="K54" s="6"/>
-      <c r="L54" s="6"/>
-      <c r="M54" s="6"/>
-      <c r="N54" s="6"/>
-      <c r="O54" s="6"/>
-      <c r="P54" s="6"/>
-      <c r="Q54" s="6"/>
-      <c r="R54" s="6"/>
-      <c r="S54" s="6"/>
-      <c r="T54" s="6"/>
-      <c r="U54" s="6"/>
-      <c r="V54" s="6"/>
-      <c r="W54" s="6"/>
-      <c r="X54" s="6"/>
-      <c r="Y54" s="6"/>
-      <c r="Z54" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6"/>
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
+      <c r="P53" s="6"/>
+      <c r="Q53" s="6"/>
+      <c r="R53" s="6"/>
+      <c r="S53" s="6"/>
+      <c r="T53" s="6"/>
+      <c r="U53" s="6"/>
+      <c r="V53" s="6"/>
+      <c r="W53" s="6"/>
+      <c r="X53" s="6"/>
+      <c r="Y53" s="6"/>
+      <c r="Z53" s="6"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A54" s="6"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
@@ -1991,8 +1981,8 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="6"/>
-      <c r="B110" s="7"/>
-      <c r="C110" s="7"/>
+      <c r="B110" s="5"/>
+      <c r="C110" s="5"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="6"/>
@@ -6443,11 +6433,6 @@
       <c r="A1000" s="6"/>
       <c r="B1000" s="5"/>
       <c r="C1000" s="5"/>
-    </row>
-    <row r="1001" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1001" s="6"/>
-      <c r="B1001" s="5"/>
-      <c r="C1001" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>